<commit_message>
cleanup environment.yml and test it
</commit_message>
<xml_diff>
--- a/3.train_ebimage/1.random_forest/results/all_scores.xlsx
+++ b/3.train_ebimage/1.random_forest/results/all_scores.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -413,6 +413,14 @@
         <v>0.3265173954740972</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0.3293225559127213</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>